<commit_message>
Add new files for employee statistics and charts: Introduced multiple Excel files for employee statistics, added Python scripts for generating team charts, and included various images for visual representation of position distributions. Also added a new PNG file for team comparison and updated Jupyter notebooks for overfitting demonstrations.
</commit_message>
<xml_diff>
--- a/justdo/250924_홈커밍데이_자리배치도_with_position.xlsx
+++ b/justdo/250924_홈커밍데이_자리배치도_with_position.xlsx
@@ -169,6 +169,56 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>50</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5715000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>75</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5715000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3549,7 +3599,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3565,40 +3615,25 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>그룹장</t>
+          <t>담당</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>담당</t>
+          <t>책임</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>본부장</t>
+          <t>수석</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>소장</t>
+          <t>기타</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
-        <is>
-          <t>수석</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>책임</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>팀장</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
         <is>
           <t>총원</t>
         </is>
@@ -3611,28 +3646,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>6</v>
-      </c>
-      <c r="G2" t="n">
-        <v>8</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -3642,28 +3668,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G3" t="n">
-        <v>7</v>
-      </c>
-      <c r="H3" t="n">
-        <v>4</v>
-      </c>
-      <c r="I3" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -3673,28 +3690,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>5</v>
-      </c>
-      <c r="G4" t="n">
-        <v>9</v>
-      </c>
-      <c r="H4" t="n">
-        <v>3</v>
-      </c>
-      <c r="I4" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -3704,28 +3712,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
-      </c>
-      <c r="G5" t="n">
         <v>10</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" t="n">
-        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -3735,28 +3734,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
-      </c>
-      <c r="G6" t="n">
-        <v>7</v>
-      </c>
-      <c r="H6" t="n">
-        <v>3</v>
-      </c>
-      <c r="I6" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -3766,28 +3756,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" t="n">
-        <v>11</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -3797,28 +3778,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
-      </c>
-      <c r="G8" t="n">
-        <v>11</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -3828,28 +3800,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G9" t="n">
-        <v>7</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -3859,28 +3822,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
         <v>10</v>
-      </c>
-      <c r="G10" t="n">
-        <v>6</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -3890,58 +3844,260 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" t="n">
         <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>8</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" t="n">
-        <v>5</v>
-      </c>
-      <c r="H11" t="n">
-        <v>2</v>
-      </c>
-      <c r="I11" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>전체</t>
+          <t>11조</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="D12" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
         <v>1</v>
       </c>
       <c r="F12" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12조</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13조</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" t="n">
+        <v>4</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14조</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15조</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16조</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17조</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" t="n">
+        <v>5</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>18조</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" t="n">
+        <v>4</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19조</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" t="n">
+        <v>5</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20조</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3</v>
+      </c>
+      <c r="F21" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>전체</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>51</v>
+      </c>
+      <c r="C22" t="n">
+        <v>81</v>
+      </c>
+      <c r="D22" t="n">
         <v>45</v>
       </c>
-      <c r="G12" t="n">
-        <v>81</v>
-      </c>
-      <c r="H12" t="n">
-        <v>15</v>
-      </c>
-      <c r="I12" t="n">
+      <c r="E22" t="n">
+        <v>22</v>
+      </c>
+      <c r="F22" t="n">
         <v>199</v>
       </c>
     </row>

</xml_diff>